<commit_message>
Setting up to run all together
</commit_message>
<xml_diff>
--- a/HOBO_Data/HOBO_tempProV2_logger_names.xlsx
+++ b/HOBO_Data/HOBO_tempProV2_logger_names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kag326\Documents\HolgersonLab_Helpful_Code\HOBO_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B4081F-BCD8-4B5B-AFC1-399ABFBE2DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6E2824-C76C-429D-9178-AD2D73C0A957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="405" yWindow="750" windowWidth="21600" windowHeight="11385" xr2:uid="{3CC198BB-0DF2-4641-B507-81C8D0AA20EB}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{3CC198BB-0DF2-4641-B507-81C8D0AA20EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -433,7 +433,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A2" sqref="A2:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>